<commit_message>
commit with import file
</commit_message>
<xml_diff>
--- a/flaskshop/static/uploads/language.xlsx
+++ b/flaskshop/static/uploads/language.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\flask-shop-master\flaskshop\static\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAA60BC-C7F2-42D0-9250-07EF28A84E19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCB3A71-3334-48F2-AFF7-611B8B44996A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="480" windowWidth="21600" windowHeight="11385" xr2:uid="{D161516E-A859-41C9-B7BC-B44E83DEC2A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D161516E-A859-41C9-B7BC-B44E83DEC2A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="160">
   <si>
     <t>Categories</t>
   </si>
@@ -355,13 +355,163 @@
   </si>
   <si>
     <t>בחר</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>פריט</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>כמות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מחיר </t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>סך הכל</t>
+  </si>
+  <si>
+    <t>Sub total</t>
+  </si>
+  <si>
+    <t>חשבון מוצרים</t>
+  </si>
+  <si>
+    <t>To:</t>
+  </si>
+  <si>
+    <t>אל</t>
+  </si>
+  <si>
+    <t>Delivery and Payment</t>
+  </si>
+  <si>
+    <t>משלוח ותשלום</t>
+  </si>
+  <si>
+    <t>Delivery needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">יבוצע משלוח </t>
+  </si>
+  <si>
+    <t>contact person and delivery address</t>
+  </si>
+  <si>
+    <t>איש הקשר והכתובת למשלוח</t>
+  </si>
+  <si>
+    <t>איסוף עצמי</t>
+  </si>
+  <si>
+    <t>Self picking</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>חשבונית</t>
+  </si>
+  <si>
+    <t>send</t>
+  </si>
+  <si>
+    <t>שלח</t>
+  </si>
+  <si>
+    <t>costumer details</t>
+  </si>
+  <si>
+    <t>Contact person and delivery address</t>
+  </si>
+  <si>
+    <t>פרטי לקוח</t>
+  </si>
+  <si>
+    <t>איש קשר וכתובת למשלוח</t>
+  </si>
+  <si>
+    <t>My Orders</t>
+  </si>
+  <si>
+    <t>ההזמנות שלי</t>
+  </si>
+  <si>
+    <t>My Addresses</t>
+  </si>
+  <si>
+    <t>Your Password</t>
+  </si>
+  <si>
+    <t>הכתובת שלי</t>
+  </si>
+  <si>
+    <t>שינוי סיסמא</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>שלום</t>
+  </si>
+  <si>
+    <t>Request a Password Reset</t>
+  </si>
+  <si>
+    <t>אזור איפוס סיסמא</t>
+  </si>
+  <si>
+    <t>Old Password</t>
+  </si>
+  <si>
+    <t>סיסמא ישנה</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>סיסמא חדשה</t>
+  </si>
+  <si>
+    <t>Repeat New Password</t>
+  </si>
+  <si>
+    <t>חזור על הסיסמא החדשה</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>אפס סיסמא</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>תאריך</t>
+  </si>
+  <si>
+    <t>No delivery</t>
+  </si>
+  <si>
+    <t>ללא משלוח</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +525,11 @@
       <color rgb="FFA9B7C6"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF91699C"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -397,11 +552,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED17F14-EF2B-4A00-A544-E664C5FAB3A5}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1124,7 +1280,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:10">
       <c r="B49" t="s">
         <v>92</v>
       </c>
@@ -1132,7 +1288,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:10">
       <c r="B50" s="1" t="s">
         <v>94</v>
       </c>
@@ -1140,7 +1296,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:10">
       <c r="B51" t="s">
         <v>96</v>
       </c>
@@ -1148,7 +1304,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:10">
       <c r="B52" t="s">
         <v>98</v>
       </c>
@@ -1156,7 +1312,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="2:3">
+    <row r="53" spans="2:10">
       <c r="B53" t="s">
         <v>100</v>
       </c>
@@ -1164,15 +1320,18 @@
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="2:3">
+    <row r="54" spans="2:10">
       <c r="B54" t="s">
         <v>102</v>
       </c>
       <c r="C54" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="55" spans="2:3">
+      <c r="J54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
       <c r="B55" t="s">
         <v>104</v>
       </c>
@@ -1180,7 +1339,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="2:3">
+    <row r="56" spans="2:10">
       <c r="B56" t="s">
         <v>106</v>
       </c>
@@ -1188,12 +1347,228 @@
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="2:3">
+    <row r="57" spans="2:10">
       <c r="B57" t="s">
         <v>108</v>
       </c>
       <c r="C57" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="B59" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="B60" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" t="s">
+        <v>126</v>
+      </c>
+      <c r="C66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="15">
+      <c r="B67" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="B68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="B69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="B70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" t="s">
+        <v>134</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
+      <c r="B72" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
+      <c r="B76" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C76" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="B79" t="s">
+        <v>150</v>
+      </c>
+      <c r="C79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="B80" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" t="s">
+        <v>34</v>
+      </c>
+      <c r="C83" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost final- all functionality added
</commit_message>
<xml_diff>
--- a/flaskshop/static/uploads/language.xlsx
+++ b/flaskshop/static/uploads/language.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\PycharmProjects\flask-shop-master\flaskshop\static\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\flask-shop\flask-shop-master\flaskshop\static\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED29344D-656F-42E0-99DF-203595BACC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C1BDFE-425A-4D78-B62B-E6574A5681E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{D161516E-A859-41C9-B7BC-B44E83DEC2A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D161516E-A859-41C9-B7BC-B44E83DEC2A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="204">
   <si>
     <t>Categories</t>
   </si>
@@ -625,6 +625,18 @@
   </si>
   <si>
     <t>on sale</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>מיוחד</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>ראה מוצר</t>
   </si>
 </sst>
 </file>
@@ -635,7 +647,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -992,16 +1004,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED17F14-EF2B-4A00-A544-E664C5FAB3A5}">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1544,7 +1556,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="2:3" ht="15">
+    <row r="67" spans="2:3" ht="15.5">
       <c r="B67" s="2" t="s">
         <v>97</v>
       </c>
@@ -1902,6 +1914,22 @@
       </c>
       <c r="C111" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3">
+      <c r="B112" t="s">
+        <v>200</v>
+      </c>
+      <c r="C112" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="B113" t="s">
+        <v>202</v>
+      </c>
+      <c r="C113" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>